<commit_message>
skripsi add penjelasan uji, uji robust fix cropping
</commit_message>
<xml_diff>
--- a/Skenario Uji Robust.xlsx
+++ b/Skenario Uji Robust.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KULIAH\SEMESTER 8\LAPORAN TA\COBA ASSEMBLE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C78E4E36-060B-42B3-8739-6965BA2BCC14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E19507-0D07-43F2-A505-B10462AA9CCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{CA13AE6D-65D7-4EC1-9E05-FC8F9DE0E163}"/>
   </bookViews>
@@ -54,18 +54,6 @@
     <t>Rotate</t>
   </si>
   <si>
-    <t>25% Horizontal</t>
-  </si>
-  <si>
-    <t>50% Horizontal</t>
-  </si>
-  <si>
-    <t>25% Vertikal</t>
-  </si>
-  <si>
-    <t>50% Vertikal</t>
-  </si>
-  <si>
     <t>Horizontal</t>
   </si>
   <si>
@@ -109,6 +97,18 @@
   </si>
   <si>
     <t>Stego Image</t>
+  </si>
+  <si>
+    <t>50% Horizontal Atas</t>
+  </si>
+  <si>
+    <t>50% Horizontal Bawah</t>
+  </si>
+  <si>
+    <t>50% Vertikal Kanan</t>
+  </si>
+  <si>
+    <t>50% Vertikal Kiri</t>
   </si>
 </sst>
 </file>
@@ -235,22 +235,10 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -262,19 +250,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -596,15 +596,15 @@
   </sheetPr>
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="67.28515625" customWidth="1"/>
-    <col min="3" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="7" width="20" customWidth="1"/>
     <col min="10" max="10" width="11.140625" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
     <col min="12" max="12" width="11.5703125" customWidth="1"/>
@@ -614,143 +614,143 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5"/>
-      <c r="W1" s="5"/>
-      <c r="X1" s="6"/>
+      <c r="B1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="8"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="A2" s="12"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="4" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="6"/>
-      <c r="N2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="O2" s="5"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="6"/>
-      <c r="S2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="6"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" s="7"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="8"/>
+      <c r="S2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="8"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="2" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="M3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="R3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="R3" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="W3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="U3" s="3" t="s">
+      <c r="X3" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -769,53 +769,56 @@
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="Q9" s="8"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="9"/>
-      <c r="V9" s="9"/>
-      <c r="W9" s="9"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="C2:C3"/>
     <mergeCell ref="C1:X1"/>
     <mergeCell ref="S2:X2"/>
     <mergeCell ref="Q2:R2"/>
@@ -823,9 +826,6 @@
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="D2:G2"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="44" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>